<commit_message>
web auth & dashboard & pages
</commit_message>
<xml_diff>
--- a/kriterii.xlsx
+++ b/kriterii.xlsx
@@ -944,7 +944,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="99">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1205,11 +1205,43 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1560,8 +1592,8 @@
   </sheetPr>
   <dimension ref="A1:L1113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A185" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D201" activeCellId="0" sqref="D201"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2567,15 +2599,15 @@
       <c r="D48" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="E48" s="27"/>
-      <c r="F48" s="29" t="s">
+      <c r="E48" s="34"/>
+      <c r="F48" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="27"/>
-      <c r="H48" s="26" t="n">
+      <c r="G48" s="34"/>
+      <c r="H48" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I48" s="66" t="n">
+      <c r="I48" s="37" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2588,15 +2620,15 @@
       <c r="D49" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="27"/>
-      <c r="F49" s="29" t="s">
+      <c r="E49" s="34"/>
+      <c r="F49" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G49" s="27"/>
-      <c r="H49" s="26" t="n">
+      <c r="G49" s="34"/>
+      <c r="H49" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I49" s="66" t="n">
+      <c r="I49" s="37" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2609,15 +2641,15 @@
       <c r="D50" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E50" s="27"/>
-      <c r="F50" s="29" t="s">
+      <c r="E50" s="34"/>
+      <c r="F50" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G50" s="27"/>
-      <c r="H50" s="26" t="n">
+      <c r="G50" s="34"/>
+      <c r="H50" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I50" s="66" t="n">
+      <c r="I50" s="37" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2630,15 +2662,15 @@
       <c r="D51" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="E51" s="27"/>
-      <c r="F51" s="29" t="s">
+      <c r="E51" s="34"/>
+      <c r="F51" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G51" s="27"/>
-      <c r="H51" s="26" t="n">
+      <c r="G51" s="34"/>
+      <c r="H51" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I51" s="66" t="n">
+      <c r="I51" s="37" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -2651,15 +2683,15 @@
       <c r="D52" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="E52" s="27"/>
-      <c r="F52" s="29" t="s">
+      <c r="E52" s="34"/>
+      <c r="F52" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G52" s="27"/>
-      <c r="H52" s="26" t="n">
+      <c r="G52" s="34"/>
+      <c r="H52" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I52" s="66" t="n">
+      <c r="I52" s="37" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -2671,12 +2703,12 @@
         <v>83</v>
       </c>
       <c r="C53" s="26"/>
-      <c r="D53" s="65"/>
+      <c r="D53" s="66"/>
       <c r="E53" s="27"/>
       <c r="F53" s="29"/>
       <c r="G53" s="27"/>
       <c r="H53" s="26"/>
-      <c r="I53" s="66"/>
+      <c r="I53" s="67"/>
     </row>
     <row r="54" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="26"/>
@@ -2684,18 +2716,18 @@
       <c r="C54" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="65" t="s">
+      <c r="D54" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="E54" s="27"/>
-      <c r="F54" s="29" t="s">
+      <c r="E54" s="52"/>
+      <c r="F54" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G54" s="27"/>
-      <c r="H54" s="26" t="n">
+      <c r="G54" s="52"/>
+      <c r="H54" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I54" s="66" t="n">
+      <c r="I54" s="55" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -2705,18 +2737,18 @@
       <c r="C55" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="65" t="s">
+      <c r="D55" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="E55" s="27"/>
-      <c r="F55" s="29" t="s">
+      <c r="E55" s="52"/>
+      <c r="F55" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G55" s="27"/>
-      <c r="H55" s="26" t="n">
+      <c r="G55" s="52"/>
+      <c r="H55" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I55" s="66" t="n">
+      <c r="I55" s="55" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -2726,18 +2758,18 @@
       <c r="C56" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="65" t="s">
+      <c r="D56" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="27"/>
-      <c r="F56" s="29" t="s">
+      <c r="E56" s="52"/>
+      <c r="F56" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G56" s="27"/>
-      <c r="H56" s="26" t="n">
+      <c r="G56" s="52"/>
+      <c r="H56" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I56" s="66" t="n">
+      <c r="I56" s="55" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -2749,12 +2781,12 @@
         <v>87</v>
       </c>
       <c r="C57" s="26"/>
-      <c r="D57" s="65"/>
+      <c r="D57" s="66"/>
       <c r="E57" s="27"/>
       <c r="F57" s="29"/>
       <c r="G57" s="27"/>
       <c r="H57" s="26"/>
-      <c r="I57" s="66"/>
+      <c r="I57" s="67"/>
     </row>
     <row r="58" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="26"/>
@@ -2762,18 +2794,18 @@
       <c r="C58" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="65" t="s">
+      <c r="D58" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="27"/>
-      <c r="F58" s="29" t="s">
+      <c r="E58" s="52"/>
+      <c r="F58" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G58" s="27"/>
-      <c r="H58" s="26" t="n">
+      <c r="G58" s="52"/>
+      <c r="H58" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I58" s="66" t="n">
+      <c r="I58" s="55" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -2783,18 +2815,18 @@
       <c r="C59" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D59" s="65" t="s">
+      <c r="D59" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="E59" s="27"/>
-      <c r="F59" s="29" t="s">
+      <c r="E59" s="52"/>
+      <c r="F59" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G59" s="27"/>
-      <c r="H59" s="26" t="n">
+      <c r="G59" s="52"/>
+      <c r="H59" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I59" s="66" t="n">
+      <c r="I59" s="55" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -2807,15 +2839,15 @@
       <c r="D60" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="E60" s="27"/>
-      <c r="F60" s="29" t="s">
+      <c r="E60" s="34"/>
+      <c r="F60" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G60" s="27"/>
-      <c r="H60" s="26" t="n">
+      <c r="G60" s="34"/>
+      <c r="H60" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I60" s="66" t="n">
+      <c r="I60" s="37" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -2827,12 +2859,12 @@
         <v>91</v>
       </c>
       <c r="C61" s="26"/>
-      <c r="D61" s="65"/>
+      <c r="D61" s="66"/>
       <c r="E61" s="27"/>
       <c r="F61" s="29"/>
       <c r="G61" s="27"/>
       <c r="H61" s="26"/>
-      <c r="I61" s="66"/>
+      <c r="I61" s="67"/>
     </row>
     <row r="62" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="26"/>
@@ -2843,15 +2875,15 @@
       <c r="D62" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="E62" s="27"/>
-      <c r="F62" s="29" t="s">
+      <c r="E62" s="34"/>
+      <c r="F62" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G62" s="27"/>
-      <c r="H62" s="26" t="n">
+      <c r="G62" s="34"/>
+      <c r="H62" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I62" s="66" t="n">
+      <c r="I62" s="37" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -2864,15 +2896,15 @@
       <c r="D63" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="E63" s="27"/>
-      <c r="F63" s="29" t="s">
+      <c r="E63" s="34"/>
+      <c r="F63" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G63" s="27"/>
-      <c r="H63" s="26" t="n">
+      <c r="G63" s="34"/>
+      <c r="H63" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I63" s="66" t="n">
+      <c r="I63" s="37" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -2882,18 +2914,18 @@
       <c r="C64" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="65" t="s">
+      <c r="D64" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="E64" s="27"/>
-      <c r="F64" s="29" t="s">
+      <c r="E64" s="52"/>
+      <c r="F64" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G64" s="27"/>
-      <c r="H64" s="26" t="n">
+      <c r="G64" s="52"/>
+      <c r="H64" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I64" s="66" t="n">
+      <c r="I64" s="55" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -2905,12 +2937,12 @@
         <v>95</v>
       </c>
       <c r="C65" s="26"/>
-      <c r="D65" s="65"/>
+      <c r="D65" s="66"/>
       <c r="E65" s="27"/>
       <c r="F65" s="29"/>
       <c r="G65" s="27"/>
       <c r="H65" s="26"/>
-      <c r="I65" s="66"/>
+      <c r="I65" s="67"/>
     </row>
     <row r="66" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="26"/>
@@ -2918,18 +2950,18 @@
       <c r="C66" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D66" s="65" t="s">
+      <c r="D66" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="E66" s="27"/>
-      <c r="F66" s="29" t="s">
+      <c r="E66" s="46"/>
+      <c r="F66" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G66" s="27"/>
-      <c r="H66" s="26" t="n">
+      <c r="G66" s="46"/>
+      <c r="H66" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="I66" s="66" t="n">
+      <c r="I66" s="49" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -2939,18 +2971,18 @@
       <c r="C67" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="65" t="s">
+      <c r="D67" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="E67" s="27"/>
-      <c r="F67" s="29" t="s">
+      <c r="E67" s="46"/>
+      <c r="F67" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G67" s="27"/>
-      <c r="H67" s="26" t="n">
+      <c r="G67" s="46"/>
+      <c r="H67" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="I67" s="66" t="n">
+      <c r="I67" s="49" t="n">
         <v>0.4</v>
       </c>
     </row>
@@ -2960,18 +2992,18 @@
       <c r="C68" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="65" t="s">
+      <c r="D68" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="E68" s="27"/>
-      <c r="F68" s="29" t="s">
+      <c r="E68" s="46"/>
+      <c r="F68" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G68" s="27"/>
-      <c r="H68" s="26" t="n">
+      <c r="G68" s="46"/>
+      <c r="H68" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="I68" s="66" t="n">
+      <c r="I68" s="49" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -2983,14 +3015,14 @@
         <v>99</v>
       </c>
       <c r="C69" s="26"/>
-      <c r="D69" s="65"/>
+      <c r="D69" s="66"/>
       <c r="E69" s="27"/>
       <c r="F69" s="29" t="s">
         <v>22</v>
       </c>
       <c r="G69" s="27"/>
       <c r="H69" s="26"/>
-      <c r="I69" s="66"/>
+      <c r="I69" s="67"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="26"/>
@@ -2998,16 +3030,16 @@
       <c r="C70" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="65" t="s">
+      <c r="D70" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="E70" s="27"/>
-      <c r="F70" s="29"/>
-      <c r="G70" s="27"/>
-      <c r="H70" s="26" t="n">
+      <c r="E70" s="52"/>
+      <c r="F70" s="53"/>
+      <c r="G70" s="52"/>
+      <c r="H70" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I70" s="66" t="n">
+      <c r="I70" s="55" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -3017,18 +3049,18 @@
       <c r="C71" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D71" s="65" t="s">
+      <c r="D71" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="E71" s="27"/>
-      <c r="F71" s="29" t="s">
+      <c r="E71" s="52"/>
+      <c r="F71" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G71" s="27"/>
-      <c r="H71" s="26" t="n">
+      <c r="G71" s="52"/>
+      <c r="H71" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I71" s="66" t="n">
+      <c r="I71" s="55" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -3038,18 +3070,18 @@
       <c r="C72" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="65" t="s">
+      <c r="D72" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="E72" s="27"/>
-      <c r="F72" s="29" t="s">
+      <c r="E72" s="52"/>
+      <c r="F72" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G72" s="27"/>
-      <c r="H72" s="26" t="n">
+      <c r="G72" s="52"/>
+      <c r="H72" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I72" s="66" t="n">
+      <c r="I72" s="55" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -3061,12 +3093,12 @@
         <v>103</v>
       </c>
       <c r="C73" s="26"/>
-      <c r="D73" s="65"/>
+      <c r="D73" s="66"/>
       <c r="E73" s="27"/>
       <c r="F73" s="29"/>
       <c r="G73" s="27"/>
       <c r="H73" s="26"/>
-      <c r="I73" s="66"/>
+      <c r="I73" s="67"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="26"/>
@@ -3074,18 +3106,18 @@
       <c r="C74" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D74" s="65" t="s">
+      <c r="D74" s="69" t="s">
         <v>104</v>
       </c>
-      <c r="E74" s="27"/>
-      <c r="F74" s="29" t="s">
+      <c r="E74" s="46"/>
+      <c r="F74" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G74" s="27"/>
-      <c r="H74" s="26" t="n">
+      <c r="G74" s="46"/>
+      <c r="H74" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="I74" s="66" t="n">
+      <c r="I74" s="49" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -3095,18 +3127,18 @@
       <c r="C75" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D75" s="65" t="s">
+      <c r="D75" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="E75" s="27"/>
-      <c r="F75" s="29" t="s">
+      <c r="E75" s="46"/>
+      <c r="F75" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G75" s="27"/>
-      <c r="H75" s="26" t="n">
+      <c r="G75" s="46"/>
+      <c r="H75" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="I75" s="66" t="n">
+      <c r="I75" s="49" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -3116,18 +3148,18 @@
       <c r="C76" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D76" s="65" t="s">
+      <c r="D76" s="69" t="s">
         <v>106</v>
       </c>
-      <c r="E76" s="27"/>
-      <c r="F76" s="29" t="s">
+      <c r="E76" s="46"/>
+      <c r="F76" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G76" s="27"/>
-      <c r="H76" s="26" t="n">
+      <c r="G76" s="46"/>
+      <c r="H76" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="I76" s="66" t="n">
+      <c r="I76" s="49" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -3137,18 +3169,18 @@
       <c r="C77" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D77" s="65" t="s">
+      <c r="D77" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="E77" s="27"/>
-      <c r="F77" s="29" t="s">
+      <c r="E77" s="46"/>
+      <c r="F77" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G77" s="27"/>
-      <c r="H77" s="26" t="n">
+      <c r="G77" s="46"/>
+      <c r="H77" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="I77" s="66" t="n">
+      <c r="I77" s="49" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -3158,18 +3190,18 @@
       <c r="C78" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D78" s="65" t="s">
+      <c r="D78" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="E78" s="27"/>
-      <c r="F78" s="29" t="s">
+      <c r="E78" s="71"/>
+      <c r="F78" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="G78" s="27"/>
-      <c r="H78" s="26" t="n">
+      <c r="G78" s="71"/>
+      <c r="H78" s="73" t="n">
         <v>2</v>
       </c>
-      <c r="I78" s="66" t="n">
+      <c r="I78" s="74" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -3179,18 +3211,18 @@
       <c r="C79" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D79" s="65" t="s">
+      <c r="D79" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="E79" s="27"/>
-      <c r="F79" s="29" t="s">
+      <c r="E79" s="52"/>
+      <c r="F79" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G79" s="27"/>
-      <c r="H79" s="26" t="n">
+      <c r="G79" s="52"/>
+      <c r="H79" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I79" s="66" t="n">
+      <c r="I79" s="55" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -3200,18 +3232,18 @@
       <c r="C80" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D80" s="65" t="s">
+      <c r="D80" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="E80" s="27"/>
-      <c r="F80" s="29" t="s">
+      <c r="E80" s="52"/>
+      <c r="F80" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G80" s="27"/>
-      <c r="H80" s="26" t="n">
+      <c r="G80" s="52"/>
+      <c r="H80" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I80" s="66" t="n">
+      <c r="I80" s="55" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -3221,18 +3253,18 @@
       <c r="C81" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D81" s="65" t="s">
+      <c r="D81" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="E81" s="27"/>
-      <c r="F81" s="29" t="s">
+      <c r="E81" s="52"/>
+      <c r="F81" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G81" s="27"/>
-      <c r="H81" s="26" t="n">
+      <c r="G81" s="52"/>
+      <c r="H81" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I81" s="66" t="n">
+      <c r="I81" s="55" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -3242,18 +3274,18 @@
       <c r="C82" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="65" t="s">
+      <c r="D82" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="E82" s="27"/>
-      <c r="F82" s="29" t="s">
+      <c r="E82" s="52"/>
+      <c r="F82" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G82" s="27"/>
-      <c r="H82" s="26" t="n">
+      <c r="G82" s="52"/>
+      <c r="H82" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I82" s="66" t="n">
+      <c r="I82" s="55" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -3263,18 +3295,18 @@
       <c r="C83" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D83" s="67" t="s">
+      <c r="D83" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="E83" s="31"/>
-      <c r="F83" s="41" t="s">
+      <c r="E83" s="52"/>
+      <c r="F83" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G83" s="31"/>
-      <c r="H83" s="30" t="n">
+      <c r="G83" s="52"/>
+      <c r="H83" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="I83" s="61" t="n">
+      <c r="I83" s="55" t="n">
         <v>0.5</v>
       </c>
       <c r="L83" s="39"/>
@@ -3287,7 +3319,7 @@
         <v>114</v>
       </c>
       <c r="C84" s="30"/>
-      <c r="D84" s="67"/>
+      <c r="D84" s="75"/>
       <c r="E84" s="31"/>
       <c r="F84" s="41"/>
       <c r="G84" s="31"/>
@@ -3301,18 +3333,18 @@
       <c r="C85" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D85" s="67" t="s">
+      <c r="D85" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="E85" s="31"/>
-      <c r="F85" s="41" t="s">
+      <c r="E85" s="34"/>
+      <c r="F85" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G85" s="31"/>
-      <c r="H85" s="30" t="n">
+      <c r="G85" s="34"/>
+      <c r="H85" s="36" t="n">
         <v>4</v>
       </c>
-      <c r="I85" s="61" t="n">
+      <c r="I85" s="37" t="n">
         <v>0.5</v>
       </c>
       <c r="L85" s="39"/>
@@ -3323,18 +3355,18 @@
       <c r="C86" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D86" s="67" t="s">
+      <c r="D86" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="E86" s="31"/>
-      <c r="F86" s="41" t="s">
+      <c r="E86" s="34"/>
+      <c r="F86" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G86" s="31"/>
-      <c r="H86" s="30" t="n">
+      <c r="G86" s="34"/>
+      <c r="H86" s="36" t="n">
         <v>4</v>
       </c>
-      <c r="I86" s="61" t="n">
+      <c r="I86" s="37" t="n">
         <v>0.5</v>
       </c>
       <c r="L86" s="39"/>
@@ -3345,18 +3377,18 @@
       <c r="C87" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D87" s="67" t="s">
+      <c r="D87" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="E87" s="31"/>
-      <c r="F87" s="41" t="s">
+      <c r="E87" s="46"/>
+      <c r="F87" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G87" s="31"/>
-      <c r="H87" s="30" t="n">
+      <c r="G87" s="46"/>
+      <c r="H87" s="48" t="n">
         <v>4</v>
       </c>
-      <c r="I87" s="61" t="n">
+      <c r="I87" s="49" t="n">
         <v>0.8</v>
       </c>
       <c r="L87" s="39"/>
@@ -3367,18 +3399,18 @@
       <c r="C88" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D88" s="67" t="s">
+      <c r="D88" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="E88" s="31"/>
-      <c r="F88" s="41" t="s">
+      <c r="E88" s="71"/>
+      <c r="F88" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="G88" s="31"/>
-      <c r="H88" s="30" t="n">
+      <c r="G88" s="71"/>
+      <c r="H88" s="73" t="n">
         <v>4</v>
       </c>
-      <c r="I88" s="61" t="n">
+      <c r="I88" s="74" t="n">
         <v>0.5</v>
       </c>
       <c r="L88" s="39"/>
@@ -3389,18 +3421,18 @@
       <c r="C89" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D89" s="67" t="s">
+      <c r="D89" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="E89" s="31"/>
-      <c r="F89" s="41" t="s">
+      <c r="E89" s="34"/>
+      <c r="F89" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G89" s="31"/>
-      <c r="H89" s="30" t="n">
+      <c r="G89" s="34"/>
+      <c r="H89" s="36" t="n">
         <v>4</v>
       </c>
-      <c r="I89" s="61" t="n">
+      <c r="I89" s="37" t="n">
         <v>0.7</v>
       </c>
       <c r="L89" s="39"/>
@@ -3413,7 +3445,7 @@
         <v>72</v>
       </c>
       <c r="C90" s="30"/>
-      <c r="D90" s="67"/>
+      <c r="D90" s="75"/>
       <c r="E90" s="31"/>
       <c r="F90" s="41"/>
       <c r="G90" s="31"/>
@@ -3430,13 +3462,13 @@
       <c r="D91" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="E91" s="27"/>
-      <c r="F91" s="29"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="26" t="n">
+      <c r="E91" s="34"/>
+      <c r="F91" s="35"/>
+      <c r="G91" s="34"/>
+      <c r="H91" s="36" t="n">
         <v>5</v>
       </c>
-      <c r="I91" s="26" t="n">
+      <c r="I91" s="36" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -3449,13 +3481,13 @@
       <c r="D92" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="E92" s="27"/>
-      <c r="F92" s="29"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="26" t="n">
+      <c r="E92" s="34"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="34"/>
+      <c r="H92" s="36" t="n">
         <v>5</v>
       </c>
-      <c r="I92" s="26" t="n">
+      <c r="I92" s="36" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -3488,11 +3520,11 @@
       </c>
       <c r="C94" s="27"/>
       <c r="D94" s="28"/>
-      <c r="E94" s="68"/>
+      <c r="E94" s="76"/>
       <c r="F94" s="29"/>
-      <c r="G94" s="68"/>
-      <c r="H94" s="68"/>
-      <c r="I94" s="68"/>
+      <c r="G94" s="76"/>
+      <c r="H94" s="76"/>
+      <c r="I94" s="76"/>
     </row>
     <row r="95" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="30"/>
@@ -3976,7 +4008,7 @@
       <c r="C118" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D118" s="67" t="s">
+      <c r="D118" s="75" t="s">
         <v>146</v>
       </c>
       <c r="E118" s="43"/>
@@ -4047,7 +4079,7 @@
       <c r="H121" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="I121" s="69" t="n">
+      <c r="I121" s="77" t="n">
         <v>0.8</v>
       </c>
       <c r="L121" s="39"/>
@@ -4069,7 +4101,7 @@
       <c r="H122" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="I122" s="69" t="n">
+      <c r="I122" s="77" t="n">
         <v>0.8</v>
       </c>
       <c r="L122" s="39"/>
@@ -4091,7 +4123,7 @@
       <c r="H123" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="I123" s="69" t="n">
+      <c r="I123" s="77" t="n">
         <v>0.8</v>
       </c>
       <c r="L123" s="39"/>
@@ -4113,7 +4145,7 @@
       <c r="H124" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="I124" s="69" t="n">
+      <c r="I124" s="77" t="n">
         <v>0.8</v>
       </c>
       <c r="L124" s="39"/>
@@ -4135,7 +4167,7 @@
       <c r="H125" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="I125" s="69" t="n">
+      <c r="I125" s="77" t="n">
         <v>0.8</v>
       </c>
       <c r="L125" s="39"/>
@@ -4157,7 +4189,7 @@
       <c r="H126" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="I126" s="69" t="n">
+      <c r="I126" s="77" t="n">
         <v>0.8</v>
       </c>
       <c r="L126" s="39"/>
@@ -4179,7 +4211,7 @@
       <c r="H127" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="I127" s="69" t="n">
+      <c r="I127" s="77" t="n">
         <v>0.5</v>
       </c>
       <c r="L127" s="39"/>
@@ -4201,7 +4233,7 @@
       <c r="H128" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="I128" s="69" t="n">
+      <c r="I128" s="77" t="n">
         <v>0.5</v>
       </c>
       <c r="L128" s="39"/>
@@ -4245,15 +4277,15 @@
     <row r="131" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="26"/>
       <c r="B131" s="27"/>
-      <c r="C131" s="70" t="s">
+      <c r="C131" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D131" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E131" s="68"/>
+      <c r="E131" s="76"/>
       <c r="F131" s="29"/>
-      <c r="G131" s="68"/>
+      <c r="G131" s="76"/>
       <c r="H131" s="26" t="n">
         <v>5</v>
       </c>
@@ -4280,27 +4312,27 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="71" t="n">
+      <c r="A133" s="79" t="n">
         <v>1</v>
       </c>
       <c r="B133" s="27" t="s">
         <v>159</v>
       </c>
       <c r="C133" s="27"/>
-      <c r="D133" s="65"/>
+      <c r="D133" s="66"/>
       <c r="E133" s="27"/>
       <c r="F133" s="29"/>
-      <c r="G133" s="68"/>
-      <c r="H133" s="68"/>
-      <c r="I133" s="68"/>
+      <c r="G133" s="76"/>
+      <c r="H133" s="76"/>
+      <c r="I133" s="76"/>
     </row>
     <row r="134" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="72"/>
+      <c r="A134" s="80"/>
       <c r="B134" s="31"/>
       <c r="C134" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D134" s="67" t="s">
+      <c r="D134" s="75" t="s">
         <v>160</v>
       </c>
       <c r="E134" s="31"/>
@@ -4315,12 +4347,12 @@
       <c r="L134" s="39"/>
     </row>
     <row r="135" s="38" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="72"/>
+      <c r="A135" s="80"/>
       <c r="B135" s="31"/>
       <c r="C135" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D135" s="67" t="s">
+      <c r="D135" s="75" t="s">
         <v>161</v>
       </c>
       <c r="E135" s="31"/>
@@ -4335,12 +4367,12 @@
       <c r="L135" s="39"/>
     </row>
     <row r="136" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="72"/>
+      <c r="A136" s="80"/>
       <c r="B136" s="31"/>
       <c r="C136" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D136" s="67" t="s">
+      <c r="D136" s="75" t="s">
         <v>162</v>
       </c>
       <c r="E136" s="31"/>
@@ -4355,12 +4387,12 @@
       <c r="L136" s="39"/>
     </row>
     <row r="137" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="72"/>
+      <c r="A137" s="80"/>
       <c r="B137" s="31"/>
       <c r="C137" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D137" s="67" t="s">
+      <c r="D137" s="75" t="s">
         <v>163</v>
       </c>
       <c r="E137" s="31"/>
@@ -4375,12 +4407,12 @@
       <c r="L137" s="39"/>
     </row>
     <row r="138" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="72"/>
+      <c r="A138" s="80"/>
       <c r="B138" s="31"/>
       <c r="C138" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D138" s="67" t="s">
+      <c r="D138" s="75" t="s">
         <v>164</v>
       </c>
       <c r="E138" s="31"/>
@@ -4395,12 +4427,12 @@
       <c r="L138" s="39"/>
     </row>
     <row r="139" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="72"/>
+      <c r="A139" s="80"/>
       <c r="B139" s="31"/>
       <c r="C139" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D139" s="67" t="s">
+      <c r="D139" s="75" t="s">
         <v>165</v>
       </c>
       <c r="E139" s="31"/>
@@ -4415,12 +4447,12 @@
       <c r="L139" s="39"/>
     </row>
     <row r="140" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="72"/>
+      <c r="A140" s="80"/>
       <c r="B140" s="31"/>
       <c r="C140" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D140" s="67" t="s">
+      <c r="D140" s="75" t="s">
         <v>166</v>
       </c>
       <c r="E140" s="31"/>
@@ -4435,12 +4467,12 @@
       <c r="L140" s="39"/>
     </row>
     <row r="141" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="72"/>
+      <c r="A141" s="80"/>
       <c r="B141" s="31"/>
       <c r="C141" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D141" s="67" t="s">
+      <c r="D141" s="75" t="s">
         <v>167</v>
       </c>
       <c r="E141" s="31"/>
@@ -4455,14 +4487,14 @@
       <c r="L141" s="39"/>
     </row>
     <row r="142" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="72" t="n">
+      <c r="A142" s="80" t="n">
         <v>2</v>
       </c>
       <c r="B142" s="31" t="s">
         <v>168</v>
       </c>
       <c r="C142" s="32"/>
-      <c r="D142" s="67"/>
+      <c r="D142" s="75"/>
       <c r="E142" s="31"/>
       <c r="F142" s="41"/>
       <c r="G142" s="43"/>
@@ -4471,12 +4503,12 @@
       <c r="L142" s="39"/>
     </row>
     <row r="143" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="72"/>
+      <c r="A143" s="80"/>
       <c r="B143" s="31"/>
       <c r="C143" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D143" s="67" t="s">
+      <c r="D143" s="75" t="s">
         <v>169</v>
       </c>
       <c r="E143" s="31"/>
@@ -4491,12 +4523,12 @@
       <c r="L143" s="39"/>
     </row>
     <row r="144" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="72"/>
+      <c r="A144" s="80"/>
       <c r="B144" s="31"/>
       <c r="C144" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D144" s="67" t="s">
+      <c r="D144" s="75" t="s">
         <v>170</v>
       </c>
       <c r="E144" s="31"/>
@@ -4511,12 +4543,12 @@
       <c r="L144" s="39"/>
     </row>
     <row r="145" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="72"/>
+      <c r="A145" s="80"/>
       <c r="B145" s="31"/>
       <c r="C145" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D145" s="67" t="s">
+      <c r="D145" s="75" t="s">
         <v>171</v>
       </c>
       <c r="E145" s="31"/>
@@ -4531,12 +4563,12 @@
       <c r="L145" s="39"/>
     </row>
     <row r="146" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="72"/>
+      <c r="A146" s="80"/>
       <c r="B146" s="31"/>
       <c r="C146" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D146" s="67" t="s">
+      <c r="D146" s="75" t="s">
         <v>172</v>
       </c>
       <c r="E146" s="31"/>
@@ -4551,14 +4583,14 @@
       <c r="L146" s="39"/>
     </row>
     <row r="147" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="72" t="n">
+      <c r="A147" s="80" t="n">
         <v>3</v>
       </c>
       <c r="B147" s="31" t="s">
         <v>173</v>
       </c>
       <c r="C147" s="32"/>
-      <c r="D147" s="67"/>
+      <c r="D147" s="75"/>
       <c r="E147" s="31"/>
       <c r="F147" s="41"/>
       <c r="G147" s="43"/>
@@ -4567,12 +4599,12 @@
       <c r="L147" s="39"/>
     </row>
     <row r="148" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="72"/>
+      <c r="A148" s="80"/>
       <c r="B148" s="31"/>
       <c r="C148" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D148" s="67" t="s">
+      <c r="D148" s="75" t="s">
         <v>174</v>
       </c>
       <c r="E148" s="31"/>
@@ -4587,12 +4619,12 @@
       <c r="L148" s="39"/>
     </row>
     <row r="149" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="72"/>
+      <c r="A149" s="80"/>
       <c r="B149" s="31"/>
       <c r="C149" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D149" s="67" t="s">
+      <c r="D149" s="75" t="s">
         <v>175</v>
       </c>
       <c r="E149" s="31"/>
@@ -4607,12 +4639,12 @@
       <c r="L149" s="39"/>
     </row>
     <row r="150" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="72"/>
+      <c r="A150" s="80"/>
       <c r="B150" s="31"/>
       <c r="C150" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D150" s="67" t="s">
+      <c r="D150" s="75" t="s">
         <v>176</v>
       </c>
       <c r="E150" s="31"/>
@@ -4627,12 +4659,12 @@
       <c r="L150" s="39"/>
     </row>
     <row r="151" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="72"/>
+      <c r="A151" s="80"/>
       <c r="B151" s="31"/>
       <c r="C151" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D151" s="67" t="s">
+      <c r="D151" s="75" t="s">
         <v>177</v>
       </c>
       <c r="E151" s="31"/>
@@ -4647,14 +4679,14 @@
       <c r="L151" s="39"/>
     </row>
     <row r="152" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="72" t="n">
+      <c r="A152" s="80" t="n">
         <v>4</v>
       </c>
       <c r="B152" s="31" t="s">
         <v>178</v>
       </c>
       <c r="C152" s="32"/>
-      <c r="D152" s="67"/>
+      <c r="D152" s="75"/>
       <c r="E152" s="31"/>
       <c r="F152" s="41"/>
       <c r="G152" s="43"/>
@@ -4663,18 +4695,18 @@
       <c r="L152" s="39"/>
     </row>
     <row r="153" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="72"/>
+      <c r="A153" s="80"/>
       <c r="B153" s="31"/>
       <c r="C153" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D153" s="67" t="s">
+      <c r="D153" s="75" t="s">
         <v>179</v>
       </c>
       <c r="E153" s="31"/>
       <c r="F153" s="41"/>
-      <c r="G153" s="67"/>
-      <c r="H153" s="72" t="n">
+      <c r="G153" s="75"/>
+      <c r="H153" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I153" s="61" t="n">
@@ -4683,18 +4715,18 @@
       <c r="L153" s="39"/>
     </row>
     <row r="154" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="72"/>
+      <c r="A154" s="80"/>
       <c r="B154" s="31"/>
       <c r="C154" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D154" s="67" t="s">
+      <c r="D154" s="75" t="s">
         <v>180</v>
       </c>
       <c r="E154" s="31"/>
-      <c r="F154" s="73"/>
-      <c r="G154" s="67"/>
-      <c r="H154" s="72" t="n">
+      <c r="F154" s="81"/>
+      <c r="G154" s="75"/>
+      <c r="H154" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I154" s="61" t="n">
@@ -4703,18 +4735,18 @@
       <c r="L154" s="39"/>
     </row>
     <row r="155" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="72"/>
+      <c r="A155" s="80"/>
       <c r="B155" s="31"/>
       <c r="C155" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D155" s="67" t="s">
+      <c r="D155" s="75" t="s">
         <v>181</v>
       </c>
       <c r="E155" s="31"/>
-      <c r="F155" s="73"/>
-      <c r="G155" s="67"/>
-      <c r="H155" s="72" t="n">
+      <c r="F155" s="81"/>
+      <c r="G155" s="75"/>
+      <c r="H155" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I155" s="61" t="n">
@@ -4723,18 +4755,18 @@
       <c r="L155" s="39"/>
     </row>
     <row r="156" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="72"/>
+      <c r="A156" s="80"/>
       <c r="B156" s="31"/>
       <c r="C156" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D156" s="67" t="s">
+      <c r="D156" s="75" t="s">
         <v>182</v>
       </c>
       <c r="E156" s="31"/>
-      <c r="F156" s="73"/>
-      <c r="G156" s="67"/>
-      <c r="H156" s="72" t="n">
+      <c r="F156" s="81"/>
+      <c r="G156" s="75"/>
+      <c r="H156" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I156" s="61" t="n">
@@ -4743,18 +4775,18 @@
       <c r="L156" s="39"/>
     </row>
     <row r="157" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="72"/>
+      <c r="A157" s="80"/>
       <c r="B157" s="31"/>
       <c r="C157" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D157" s="67" t="s">
+      <c r="D157" s="75" t="s">
         <v>183</v>
       </c>
       <c r="E157" s="31"/>
-      <c r="F157" s="73"/>
-      <c r="G157" s="67"/>
-      <c r="H157" s="72" t="n">
+      <c r="F157" s="81"/>
+      <c r="G157" s="75"/>
+      <c r="H157" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I157" s="61" t="n">
@@ -4763,18 +4795,18 @@
       <c r="L157" s="39"/>
     </row>
     <row r="158" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="72"/>
+      <c r="A158" s="80"/>
       <c r="B158" s="31"/>
       <c r="C158" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D158" s="67" t="s">
+      <c r="D158" s="75" t="s">
         <v>184</v>
       </c>
       <c r="E158" s="31"/>
       <c r="F158" s="41"/>
-      <c r="G158" s="67"/>
-      <c r="H158" s="72" t="n">
+      <c r="G158" s="75"/>
+      <c r="H158" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I158" s="61" t="n">
@@ -4783,18 +4815,18 @@
       <c r="L158" s="39"/>
     </row>
     <row r="159" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="72"/>
+      <c r="A159" s="80"/>
       <c r="B159" s="31"/>
       <c r="C159" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D159" s="67" t="s">
+      <c r="D159" s="75" t="s">
         <v>185</v>
       </c>
       <c r="E159" s="31"/>
       <c r="F159" s="41"/>
-      <c r="G159" s="67"/>
-      <c r="H159" s="72" t="n">
+      <c r="G159" s="75"/>
+      <c r="H159" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I159" s="61" t="n">
@@ -4803,34 +4835,34 @@
       <c r="L159" s="39"/>
     </row>
     <row r="160" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="72" t="n">
+      <c r="A160" s="80" t="n">
         <v>5</v>
       </c>
       <c r="B160" s="31" t="s">
         <v>186</v>
       </c>
       <c r="C160" s="32"/>
-      <c r="D160" s="67"/>
+      <c r="D160" s="75"/>
       <c r="E160" s="31"/>
       <c r="F160" s="41"/>
-      <c r="G160" s="67"/>
-      <c r="H160" s="72"/>
+      <c r="G160" s="75"/>
+      <c r="H160" s="80"/>
       <c r="I160" s="61"/>
       <c r="L160" s="39"/>
     </row>
     <row r="161" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="72"/>
+      <c r="A161" s="80"/>
       <c r="B161" s="31"/>
       <c r="C161" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D161" s="67" t="s">
+      <c r="D161" s="75" t="s">
         <v>187</v>
       </c>
       <c r="E161" s="31"/>
       <c r="F161" s="41"/>
-      <c r="G161" s="67"/>
-      <c r="H161" s="72" t="n">
+      <c r="G161" s="75"/>
+      <c r="H161" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I161" s="61" t="n">
@@ -4839,18 +4871,18 @@
       <c r="L161" s="39"/>
     </row>
     <row r="162" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="72"/>
+      <c r="A162" s="80"/>
       <c r="B162" s="31"/>
       <c r="C162" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D162" s="67" t="s">
+      <c r="D162" s="75" t="s">
         <v>188</v>
       </c>
       <c r="E162" s="31"/>
       <c r="F162" s="41"/>
-      <c r="G162" s="67"/>
-      <c r="H162" s="72" t="n">
+      <c r="G162" s="75"/>
+      <c r="H162" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I162" s="61" t="n">
@@ -4859,18 +4891,18 @@
       <c r="L162" s="39"/>
     </row>
     <row r="163" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="72"/>
+      <c r="A163" s="80"/>
       <c r="B163" s="31"/>
       <c r="C163" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D163" s="67" t="s">
+      <c r="D163" s="75" t="s">
         <v>189</v>
       </c>
       <c r="E163" s="31"/>
       <c r="F163" s="41"/>
-      <c r="G163" s="67"/>
-      <c r="H163" s="72" t="n">
+      <c r="G163" s="75"/>
+      <c r="H163" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I163" s="61" t="n">
@@ -4879,18 +4911,18 @@
       <c r="L163" s="39"/>
     </row>
     <row r="164" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="72"/>
+      <c r="A164" s="80"/>
       <c r="B164" s="31"/>
       <c r="C164" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D164" s="67" t="s">
+      <c r="D164" s="75" t="s">
         <v>190</v>
       </c>
       <c r="E164" s="31"/>
       <c r="F164" s="41"/>
-      <c r="G164" s="67"/>
-      <c r="H164" s="72" t="n">
+      <c r="G164" s="75"/>
+      <c r="H164" s="80" t="n">
         <v>2</v>
       </c>
       <c r="I164" s="61" t="n">
@@ -4899,18 +4931,18 @@
       <c r="L164" s="39"/>
     </row>
     <row r="165" s="38" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="72"/>
+      <c r="A165" s="80"/>
       <c r="B165" s="31"/>
       <c r="C165" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D165" s="67" t="s">
+      <c r="D165" s="75" t="s">
         <v>191</v>
       </c>
       <c r="E165" s="31"/>
       <c r="F165" s="41"/>
-      <c r="G165" s="67"/>
-      <c r="H165" s="72" t="n">
+      <c r="G165" s="75"/>
+      <c r="H165" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I165" s="61" t="n">
@@ -4919,189 +4951,189 @@
       <c r="L165" s="39"/>
     </row>
     <row r="166" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="71"/>
+      <c r="A166" s="79"/>
       <c r="B166" s="27"/>
-      <c r="C166" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D166" s="65" t="s">
+      <c r="C166" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D166" s="66" t="s">
         <v>192</v>
       </c>
       <c r="E166" s="27"/>
       <c r="F166" s="29"/>
-      <c r="G166" s="65"/>
-      <c r="H166" s="71" t="n">
+      <c r="G166" s="66"/>
+      <c r="H166" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="I166" s="66" t="n">
+      <c r="I166" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="71"/>
+      <c r="A167" s="79"/>
       <c r="B167" s="27"/>
-      <c r="C167" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D167" s="65" t="s">
+      <c r="C167" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D167" s="66" t="s">
         <v>193</v>
       </c>
       <c r="E167" s="27"/>
       <c r="F167" s="29"/>
-      <c r="G167" s="65"/>
-      <c r="H167" s="71" t="n">
+      <c r="G167" s="66"/>
+      <c r="H167" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="I167" s="66" t="n">
+      <c r="I167" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="71" t="n">
+      <c r="A168" s="79" t="n">
         <v>6</v>
       </c>
       <c r="B168" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="C168" s="70"/>
-      <c r="D168" s="65"/>
+      <c r="C168" s="78"/>
+      <c r="D168" s="66"/>
       <c r="E168" s="27"/>
       <c r="F168" s="29"/>
-      <c r="G168" s="65"/>
-      <c r="H168" s="71"/>
-      <c r="I168" s="66"/>
+      <c r="G168" s="66"/>
+      <c r="H168" s="79"/>
+      <c r="I168" s="67"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="71"/>
+      <c r="A169" s="79"/>
       <c r="B169" s="27"/>
-      <c r="C169" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D169" s="65" t="s">
+      <c r="C169" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D169" s="66" t="s">
         <v>195</v>
       </c>
       <c r="E169" s="27"/>
       <c r="F169" s="29"/>
-      <c r="G169" s="65"/>
-      <c r="H169" s="71" t="n">
+      <c r="G169" s="66"/>
+      <c r="H169" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="I169" s="66" t="n">
+      <c r="I169" s="67" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="71"/>
+      <c r="A170" s="79"/>
       <c r="B170" s="27"/>
-      <c r="C170" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D170" s="65" t="s">
+      <c r="C170" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D170" s="66" t="s">
         <v>196</v>
       </c>
       <c r="E170" s="27"/>
       <c r="F170" s="29"/>
-      <c r="G170" s="65"/>
-      <c r="H170" s="71" t="n">
+      <c r="G170" s="66"/>
+      <c r="H170" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="I170" s="66" t="n">
+      <c r="I170" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="71"/>
+      <c r="A171" s="79"/>
       <c r="B171" s="27"/>
-      <c r="C171" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D171" s="65" t="s">
+      <c r="C171" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D171" s="66" t="s">
         <v>197</v>
       </c>
       <c r="E171" s="27"/>
       <c r="F171" s="29"/>
-      <c r="G171" s="65"/>
-      <c r="H171" s="71" t="n">
+      <c r="G171" s="66"/>
+      <c r="H171" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="I171" s="66" t="n">
+      <c r="I171" s="67" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="71"/>
+      <c r="A172" s="79"/>
       <c r="B172" s="27"/>
-      <c r="C172" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D172" s="65" t="s">
+      <c r="C172" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D172" s="66" t="s">
         <v>198</v>
       </c>
       <c r="E172" s="27"/>
       <c r="F172" s="29"/>
-      <c r="G172" s="65"/>
-      <c r="H172" s="71" t="n">
+      <c r="G172" s="66"/>
+      <c r="H172" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="I172" s="66" t="n">
+      <c r="I172" s="67" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="71"/>
+      <c r="A173" s="79"/>
       <c r="B173" s="27"/>
-      <c r="C173" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D173" s="65" t="s">
+      <c r="C173" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D173" s="66" t="s">
         <v>199</v>
       </c>
       <c r="E173" s="27"/>
       <c r="F173" s="29"/>
-      <c r="G173" s="65"/>
-      <c r="H173" s="71" t="n">
+      <c r="G173" s="66"/>
+      <c r="H173" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="I173" s="66" t="n">
+      <c r="I173" s="67" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="71"/>
+      <c r="A174" s="79"/>
       <c r="B174" s="27"/>
-      <c r="C174" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="D174" s="65" t="s">
+      <c r="C174" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D174" s="66" t="s">
         <v>200</v>
       </c>
       <c r="E174" s="27"/>
-      <c r="F174" s="74"/>
-      <c r="G174" s="65"/>
-      <c r="H174" s="71" t="n">
+      <c r="F174" s="82"/>
+      <c r="G174" s="66"/>
+      <c r="H174" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="I174" s="66" t="n">
+      <c r="I174" s="67" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="71" t="n">
+      <c r="A175" s="79" t="n">
         <v>7</v>
       </c>
       <c r="B175" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="C175" s="70"/>
-      <c r="D175" s="65"/>
+      <c r="C175" s="78"/>
+      <c r="D175" s="66"/>
       <c r="E175" s="27"/>
-      <c r="F175" s="74"/>
-      <c r="G175" s="65"/>
-      <c r="H175" s="71"/>
-      <c r="I175" s="66"/>
+      <c r="F175" s="82"/>
+      <c r="G175" s="66"/>
+      <c r="H175" s="79"/>
+      <c r="I175" s="67"/>
     </row>
     <row r="176" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="72"/>
+      <c r="A176" s="80"/>
       <c r="B176" s="31"/>
       <c r="C176" s="32" t="s">
         <v>20</v>
@@ -5110,9 +5142,9 @@
         <v>201</v>
       </c>
       <c r="E176" s="31"/>
-      <c r="F176" s="73"/>
-      <c r="G176" s="67"/>
-      <c r="H176" s="72" t="n">
+      <c r="F176" s="81"/>
+      <c r="G176" s="75"/>
+      <c r="H176" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I176" s="61" t="n">
@@ -5121,7 +5153,7 @@
       <c r="L176" s="39"/>
     </row>
     <row r="177" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="72"/>
+      <c r="A177" s="80"/>
       <c r="B177" s="31"/>
       <c r="C177" s="32" t="s">
         <v>20</v>
@@ -5131,8 +5163,8 @@
       </c>
       <c r="E177" s="31"/>
       <c r="F177" s="41"/>
-      <c r="G177" s="67"/>
-      <c r="H177" s="72" t="n">
+      <c r="G177" s="75"/>
+      <c r="H177" s="80" t="n">
         <v>3</v>
       </c>
       <c r="I177" s="61" t="n">
@@ -5141,7 +5173,7 @@
       <c r="L177" s="39"/>
     </row>
     <row r="178" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="72"/>
+      <c r="A178" s="80"/>
       <c r="B178" s="31"/>
       <c r="C178" s="32" t="s">
         <v>20</v>
@@ -5150,9 +5182,9 @@
         <v>203</v>
       </c>
       <c r="E178" s="31"/>
-      <c r="F178" s="73"/>
-      <c r="G178" s="67"/>
-      <c r="H178" s="72" t="n">
+      <c r="F178" s="81"/>
+      <c r="G178" s="75"/>
+      <c r="H178" s="80" t="n">
         <v>4</v>
       </c>
       <c r="I178" s="61" t="n">
@@ -5161,7 +5193,7 @@
       <c r="L178" s="39"/>
     </row>
     <row r="179" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="72"/>
+      <c r="A179" s="80"/>
       <c r="B179" s="31"/>
       <c r="C179" s="32" t="s">
         <v>20</v>
@@ -5170,9 +5202,9 @@
         <v>204</v>
       </c>
       <c r="E179" s="31"/>
-      <c r="F179" s="73"/>
-      <c r="G179" s="67"/>
-      <c r="H179" s="72" t="n">
+      <c r="F179" s="81"/>
+      <c r="G179" s="75"/>
+      <c r="H179" s="80" t="n">
         <v>4</v>
       </c>
       <c r="I179" s="61" t="n">
@@ -5181,7 +5213,7 @@
       <c r="L179" s="39"/>
     </row>
     <row r="180" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="72"/>
+      <c r="A180" s="80"/>
       <c r="B180" s="31"/>
       <c r="C180" s="32" t="s">
         <v>20</v>
@@ -5190,9 +5222,9 @@
         <v>205</v>
       </c>
       <c r="E180" s="31"/>
-      <c r="F180" s="73"/>
-      <c r="G180" s="67"/>
-      <c r="H180" s="72" t="n">
+      <c r="F180" s="81"/>
+      <c r="G180" s="75"/>
+      <c r="H180" s="80" t="n">
         <v>4</v>
       </c>
       <c r="I180" s="61" t="n">
@@ -5212,14 +5244,14 @@
       <c r="E181" s="31"/>
       <c r="F181" s="41"/>
       <c r="G181" s="43"/>
-      <c r="H181" s="72"/>
+      <c r="H181" s="80"/>
       <c r="I181" s="61"/>
       <c r="L181" s="39"/>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="68"/>
+      <c r="A182" s="76"/>
       <c r="B182" s="27"/>
-      <c r="C182" s="70" t="s">
+      <c r="C182" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D182" s="28" t="s">
@@ -5227,30 +5259,30 @@
       </c>
       <c r="E182" s="27"/>
       <c r="F182" s="29"/>
-      <c r="G182" s="68"/>
-      <c r="H182" s="71" t="n">
+      <c r="G182" s="76"/>
+      <c r="H182" s="79" t="n">
         <v>5</v>
       </c>
-      <c r="I182" s="66" t="n">
+      <c r="I182" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="68"/>
+      <c r="A183" s="76"/>
       <c r="B183" s="27"/>
-      <c r="C183" s="70" t="s">
+      <c r="C183" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D183" s="28" t="s">
         <v>74</v>
       </c>
       <c r="E183" s="27"/>
-      <c r="F183" s="74"/>
-      <c r="G183" s="68"/>
+      <c r="F183" s="82"/>
+      <c r="G183" s="76"/>
       <c r="H183" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="I183" s="66" t="n">
+      <c r="I183" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -5281,66 +5313,66 @@
       </c>
       <c r="C185" s="27"/>
       <c r="D185" s="27"/>
-      <c r="E185" s="71"/>
-      <c r="F185" s="74"/>
-      <c r="G185" s="68"/>
-      <c r="H185" s="68"/>
-      <c r="I185" s="75"/>
+      <c r="E185" s="79"/>
+      <c r="F185" s="82"/>
+      <c r="G185" s="76"/>
+      <c r="H185" s="76"/>
+      <c r="I185" s="83"/>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="26"/>
       <c r="B186" s="27"/>
-      <c r="C186" s="70" t="s">
+      <c r="C186" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D186" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="E186" s="71"/>
-      <c r="F186" s="74"/>
-      <c r="G186" s="68"/>
+      <c r="E186" s="79"/>
+      <c r="F186" s="82"/>
+      <c r="G186" s="76"/>
       <c r="H186" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I186" s="66" t="n">
+      <c r="I186" s="67" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="26"/>
       <c r="B187" s="27"/>
-      <c r="C187" s="70" t="s">
+      <c r="C187" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D187" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="E187" s="71"/>
-      <c r="F187" s="74"/>
-      <c r="G187" s="68"/>
+      <c r="E187" s="79"/>
+      <c r="F187" s="82"/>
+      <c r="G187" s="76"/>
       <c r="H187" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I187" s="66" t="n">
+      <c r="I187" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="26"/>
       <c r="B188" s="27"/>
-      <c r="C188" s="70" t="s">
+      <c r="C188" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D188" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="E188" s="71"/>
-      <c r="F188" s="74"/>
-      <c r="G188" s="68"/>
+      <c r="E188" s="79"/>
+      <c r="F188" s="82"/>
+      <c r="G188" s="76"/>
       <c r="H188" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I188" s="66" t="n">
+      <c r="I188" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -5351,106 +5383,106 @@
       <c r="B189" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="C189" s="70"/>
+      <c r="C189" s="78"/>
       <c r="D189" s="27"/>
-      <c r="E189" s="71"/>
-      <c r="F189" s="74"/>
-      <c r="G189" s="68"/>
+      <c r="E189" s="79"/>
+      <c r="F189" s="82"/>
+      <c r="G189" s="76"/>
       <c r="H189" s="26"/>
-      <c r="I189" s="66"/>
+      <c r="I189" s="67"/>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="26"/>
       <c r="B190" s="27"/>
-      <c r="C190" s="70" t="s">
+      <c r="C190" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D190" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="E190" s="71"/>
-      <c r="F190" s="74"/>
-      <c r="G190" s="68"/>
+      <c r="E190" s="79"/>
+      <c r="F190" s="82"/>
+      <c r="G190" s="76"/>
       <c r="H190" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I190" s="66" t="n">
+      <c r="I190" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="26"/>
       <c r="B191" s="27"/>
-      <c r="C191" s="70" t="s">
+      <c r="C191" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D191" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="E191" s="71"/>
-      <c r="F191" s="74"/>
-      <c r="G191" s="68"/>
+      <c r="E191" s="79"/>
+      <c r="F191" s="82"/>
+      <c r="G191" s="76"/>
       <c r="H191" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I191" s="66" t="n">
+      <c r="I191" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="26"/>
       <c r="B192" s="27"/>
-      <c r="C192" s="70" t="s">
+      <c r="C192" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D192" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="E192" s="71"/>
-      <c r="F192" s="74"/>
-      <c r="G192" s="68"/>
+      <c r="E192" s="79"/>
+      <c r="F192" s="82"/>
+      <c r="G192" s="76"/>
       <c r="H192" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I192" s="66" t="n">
+      <c r="I192" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="26"/>
       <c r="B193" s="27"/>
-      <c r="C193" s="70" t="s">
+      <c r="C193" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D193" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="E193" s="71"/>
-      <c r="F193" s="74"/>
-      <c r="G193" s="68"/>
+      <c r="E193" s="79"/>
+      <c r="F193" s="82"/>
+      <c r="G193" s="76"/>
       <c r="H193" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I193" s="66" t="n">
+      <c r="I193" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="26"/>
       <c r="B194" s="27"/>
-      <c r="C194" s="70" t="s">
+      <c r="C194" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D194" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="E194" s="71"/>
-      <c r="F194" s="74"/>
-      <c r="G194" s="68"/>
+      <c r="E194" s="79"/>
+      <c r="F194" s="82"/>
+      <c r="G194" s="76"/>
       <c r="H194" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I194" s="66" t="n">
+      <c r="I194" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -5461,168 +5493,168 @@
       <c r="B195" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="C195" s="70"/>
+      <c r="C195" s="78"/>
       <c r="D195" s="27"/>
-      <c r="E195" s="71"/>
-      <c r="F195" s="74"/>
-      <c r="G195" s="68"/>
+      <c r="E195" s="79"/>
+      <c r="F195" s="82"/>
+      <c r="G195" s="76"/>
       <c r="H195" s="26"/>
-      <c r="I195" s="66"/>
+      <c r="I195" s="67"/>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="26"/>
       <c r="B196" s="27"/>
-      <c r="C196" s="70" t="s">
+      <c r="C196" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D196" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="E196" s="71"/>
-      <c r="F196" s="74"/>
-      <c r="G196" s="68"/>
+      <c r="E196" s="79"/>
+      <c r="F196" s="82"/>
+      <c r="G196" s="76"/>
       <c r="H196" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I196" s="66" t="n">
+      <c r="I196" s="67" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="26"/>
       <c r="B197" s="27"/>
-      <c r="C197" s="70" t="s">
+      <c r="C197" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D197" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="E197" s="71"/>
-      <c r="F197" s="74"/>
-      <c r="G197" s="68"/>
+      <c r="E197" s="79"/>
+      <c r="F197" s="82"/>
+      <c r="G197" s="76"/>
       <c r="H197" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I197" s="66" t="n">
+      <c r="I197" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="26"/>
       <c r="B198" s="27"/>
-      <c r="C198" s="70" t="s">
+      <c r="C198" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D198" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="E198" s="71"/>
-      <c r="F198" s="74"/>
-      <c r="G198" s="68"/>
+      <c r="E198" s="79"/>
+      <c r="F198" s="82"/>
+      <c r="G198" s="76"/>
       <c r="H198" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I198" s="66" t="n">
+      <c r="I198" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="26"/>
       <c r="B199" s="27"/>
-      <c r="C199" s="70" t="s">
+      <c r="C199" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D199" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="E199" s="71"/>
-      <c r="F199" s="74"/>
-      <c r="G199" s="68"/>
+      <c r="E199" s="79"/>
+      <c r="F199" s="82"/>
+      <c r="G199" s="76"/>
       <c r="H199" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I199" s="66" t="n">
+      <c r="I199" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="26"/>
       <c r="B200" s="27"/>
-      <c r="C200" s="70" t="s">
+      <c r="C200" s="78" t="s">
         <v>223</v>
       </c>
       <c r="D200" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="E200" s="71"/>
-      <c r="F200" s="74"/>
-      <c r="G200" s="68"/>
+      <c r="E200" s="79"/>
+      <c r="F200" s="82"/>
+      <c r="G200" s="76"/>
       <c r="H200" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="I200" s="66" t="n">
+      <c r="I200" s="67" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="26"/>
       <c r="B201" s="27"/>
-      <c r="C201" s="70"/>
+      <c r="C201" s="78"/>
       <c r="D201" s="27"/>
-      <c r="E201" s="71" t="n">
+      <c r="E201" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="F201" s="74" t="s">
+      <c r="F201" s="82" t="s">
         <v>225</v>
       </c>
-      <c r="G201" s="68"/>
+      <c r="G201" s="76"/>
       <c r="H201" s="26"/>
-      <c r="I201" s="75"/>
+      <c r="I201" s="83"/>
     </row>
     <row r="202" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="26"/>
       <c r="B202" s="27"/>
-      <c r="C202" s="70"/>
+      <c r="C202" s="78"/>
       <c r="D202" s="27"/>
-      <c r="E202" s="71" t="n">
+      <c r="E202" s="79" t="n">
         <v>1</v>
       </c>
-      <c r="F202" s="74" t="s">
+      <c r="F202" s="82" t="s">
         <v>226</v>
       </c>
-      <c r="G202" s="68"/>
-      <c r="H202" s="68"/>
-      <c r="I202" s="75"/>
+      <c r="G202" s="76"/>
+      <c r="H202" s="76"/>
+      <c r="I202" s="83"/>
     </row>
     <row r="203" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="26"/>
       <c r="B203" s="27"/>
-      <c r="C203" s="70"/>
+      <c r="C203" s="78"/>
       <c r="D203" s="27"/>
-      <c r="E203" s="71" t="n">
+      <c r="E203" s="79" t="n">
         <v>2</v>
       </c>
-      <c r="F203" s="74" t="s">
+      <c r="F203" s="82" t="s">
         <v>227</v>
       </c>
-      <c r="G203" s="68"/>
-      <c r="H203" s="68"/>
-      <c r="I203" s="75"/>
+      <c r="G203" s="76"/>
+      <c r="H203" s="76"/>
+      <c r="I203" s="83"/>
     </row>
     <row r="204" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="26"/>
       <c r="B204" s="27"/>
-      <c r="C204" s="70"/>
+      <c r="C204" s="78"/>
       <c r="D204" s="27"/>
-      <c r="E204" s="71" t="n">
+      <c r="E204" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="F204" s="74" t="s">
+      <c r="F204" s="82" t="s">
         <v>228</v>
       </c>
-      <c r="G204" s="68"/>
-      <c r="H204" s="68"/>
-      <c r="I204" s="75"/>
+      <c r="G204" s="76"/>
+      <c r="H204" s="76"/>
+      <c r="I204" s="83"/>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="26" t="n">
@@ -5631,62 +5663,62 @@
       <c r="B205" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C205" s="70"/>
+      <c r="C205" s="78"/>
       <c r="D205" s="27"/>
-      <c r="E205" s="71"/>
-      <c r="F205" s="74"/>
-      <c r="G205" s="68"/>
-      <c r="H205" s="68"/>
-      <c r="I205" s="75"/>
+      <c r="E205" s="79"/>
+      <c r="F205" s="82"/>
+      <c r="G205" s="76"/>
+      <c r="H205" s="76"/>
+      <c r="I205" s="83"/>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="68"/>
+      <c r="A206" s="76"/>
       <c r="B206" s="27"/>
-      <c r="C206" s="70" t="s">
+      <c r="C206" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D206" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="E206" s="71"/>
-      <c r="F206" s="74"/>
-      <c r="G206" s="68"/>
+      <c r="E206" s="79"/>
+      <c r="F206" s="82"/>
+      <c r="G206" s="76"/>
       <c r="H206" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="I206" s="66" t="n">
+      <c r="I206" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="68"/>
+      <c r="A207" s="76"/>
       <c r="B207" s="27"/>
-      <c r="C207" s="70" t="s">
+      <c r="C207" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D207" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E207" s="71"/>
-      <c r="F207" s="74"/>
-      <c r="G207" s="68"/>
+      <c r="E207" s="79"/>
+      <c r="F207" s="82"/>
+      <c r="G207" s="76"/>
       <c r="H207" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="I207" s="66" t="n">
+      <c r="I207" s="67" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A208" s="76"/>
-      <c r="B208" s="77"/>
-      <c r="C208" s="78"/>
-      <c r="D208" s="79"/>
-      <c r="E208" s="78"/>
-      <c r="F208" s="80" t="s">
+      <c r="A208" s="84"/>
+      <c r="B208" s="85"/>
+      <c r="C208" s="86"/>
+      <c r="D208" s="87"/>
+      <c r="E208" s="86"/>
+      <c r="F208" s="88" t="s">
         <v>231</v>
       </c>
-      <c r="G208" s="81"/>
+      <c r="G208" s="89"/>
       <c r="H208" s="18"/>
       <c r="I208" s="20" t="n">
         <f aca="false">I132+I93+I46+I6+I184</f>
@@ -8228,9 +8260,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="82" width="6.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="83" width="63.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="84" width="6.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="90" width="6.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="91" width="63.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="92" width="6.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8240,47 +8272,47 @@
       <c r="B1" s="18"/>
     </row>
     <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="85" t="n">
+      <c r="A2" s="93" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="94" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="85" t="n">
+      <c r="A3" s="93" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="94" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="85" t="n">
+      <c r="A4" s="93" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="94" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="85" t="n">
+      <c r="A5" s="93" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="94" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="85" t="n">
+      <c r="A6" s="93" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="82" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="85" t="n">
+      <c r="A7" s="93" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="29" t="s">
@@ -8314,704 +8346,704 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="84" width="26.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="84" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="84" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="92" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="92" width="26.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="92" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="92" width="8.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="87"/>
+      <c r="B1" s="95"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="88" t="n">
+      <c r="A2" s="96" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="97" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="88" t="n">
+      <c r="A3" s="96" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="97" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="88" t="n">
+      <c r="A4" s="96" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="97" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="88" t="n">
+      <c r="A5" s="96" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="97" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="88" t="n">
+      <c r="A6" s="96" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="97" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="88" t="n">
+      <c r="A7" s="96" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="97" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="90"/>
+      <c r="B8" s="98"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="90"/>
+      <c r="B9" s="98"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="90"/>
+      <c r="B10" s="98"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="90"/>
+      <c r="B11" s="98"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="90"/>
+      <c r="B12" s="98"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="90"/>
+      <c r="B13" s="98"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="90"/>
+      <c r="B14" s="98"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="90"/>
+      <c r="B15" s="98"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="90"/>
+      <c r="B16" s="98"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="90"/>
+      <c r="B17" s="98"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="90"/>
+      <c r="B18" s="98"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="90"/>
+      <c r="B19" s="98"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="90"/>
+      <c r="B20" s="98"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="90"/>
+      <c r="B21" s="98"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="90"/>
+      <c r="B22" s="98"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="90"/>
+      <c r="B23" s="98"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="90"/>
+      <c r="B24" s="98"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="90"/>
+      <c r="B25" s="98"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="90"/>
+      <c r="B26" s="98"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="90"/>
+      <c r="B27" s="98"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="90"/>
+      <c r="B28" s="98"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="90"/>
+      <c r="B29" s="98"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="90"/>
+      <c r="B30" s="98"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="90"/>
+      <c r="B31" s="98"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="90"/>
+      <c r="B32" s="98"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="90"/>
+      <c r="B33" s="98"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="90"/>
+      <c r="B34" s="98"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="90"/>
+      <c r="B35" s="98"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="90"/>
+      <c r="B36" s="98"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="90"/>
+      <c r="B37" s="98"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="90"/>
+      <c r="B38" s="98"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="90"/>
+      <c r="B39" s="98"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="90"/>
+      <c r="B40" s="98"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="90"/>
+      <c r="B41" s="98"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="90"/>
+      <c r="B42" s="98"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="90"/>
+      <c r="B43" s="98"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="90"/>
+      <c r="B44" s="98"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="90"/>
+      <c r="B45" s="98"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="90"/>
+      <c r="B46" s="98"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="90"/>
+      <c r="B47" s="98"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="90"/>
+      <c r="B48" s="98"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="90"/>
+      <c r="B49" s="98"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="90"/>
+      <c r="B50" s="98"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="90"/>
+      <c r="B51" s="98"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="90"/>
+      <c r="B52" s="98"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="90"/>
+      <c r="B53" s="98"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="90"/>
+      <c r="B54" s="98"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="90"/>
+      <c r="B55" s="98"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="90"/>
+      <c r="B56" s="98"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="90"/>
+      <c r="B57" s="98"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="90"/>
+      <c r="B58" s="98"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="90"/>
+      <c r="B59" s="98"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="90"/>
+      <c r="B60" s="98"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="90"/>
+      <c r="B61" s="98"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="90"/>
+      <c r="B62" s="98"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="90"/>
+      <c r="B63" s="98"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="90"/>
+      <c r="B64" s="98"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="90"/>
+      <c r="B65" s="98"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="90"/>
+      <c r="B66" s="98"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="90"/>
+      <c r="B67" s="98"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="90"/>
+      <c r="B68" s="98"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="90"/>
+      <c r="B69" s="98"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="90"/>
+      <c r="B70" s="98"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="90"/>
+      <c r="B71" s="98"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="90"/>
+      <c r="B72" s="98"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="90"/>
+      <c r="B73" s="98"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="90"/>
+      <c r="B74" s="98"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="90"/>
+      <c r="B75" s="98"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="90"/>
+      <c r="B76" s="98"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="90"/>
+      <c r="B77" s="98"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="90"/>
+      <c r="B78" s="98"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="90"/>
+      <c r="B79" s="98"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="90"/>
+      <c r="B80" s="98"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="90"/>
+      <c r="B81" s="98"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="90"/>
+      <c r="B82" s="98"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="90"/>
+      <c r="B83" s="98"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="90"/>
+      <c r="B84" s="98"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="90"/>
+      <c r="B85" s="98"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="90"/>
+      <c r="B86" s="98"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="90"/>
+      <c r="B87" s="98"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="90"/>
+      <c r="B88" s="98"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="90"/>
+      <c r="B89" s="98"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="90"/>
+      <c r="B90" s="98"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="90"/>
+      <c r="B91" s="98"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B92" s="90"/>
+      <c r="B92" s="98"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B93" s="90"/>
+      <c r="B93" s="98"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B94" s="90"/>
+      <c r="B94" s="98"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B95" s="90"/>
+      <c r="B95" s="98"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B96" s="90"/>
+      <c r="B96" s="98"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="90"/>
+      <c r="B97" s="98"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="90"/>
+      <c r="B98" s="98"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="90"/>
+      <c r="B99" s="98"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="90"/>
+      <c r="B100" s="98"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="90"/>
+      <c r="B101" s="98"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="90"/>
+      <c r="B102" s="98"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="90"/>
+      <c r="B103" s="98"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="90"/>
+      <c r="B104" s="98"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="90"/>
+      <c r="B105" s="98"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="90"/>
+      <c r="B106" s="98"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="90"/>
+      <c r="B107" s="98"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="90"/>
+      <c r="B108" s="98"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="90"/>
+      <c r="B109" s="98"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="90"/>
+      <c r="B110" s="98"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="90"/>
+      <c r="B111" s="98"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="90"/>
+      <c r="B112" s="98"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="90"/>
+      <c r="B113" s="98"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="90"/>
+      <c r="B114" s="98"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="90"/>
+      <c r="B115" s="98"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="90"/>
+      <c r="B116" s="98"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="90"/>
+      <c r="B117" s="98"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="90"/>
+      <c r="B118" s="98"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="90"/>
+      <c r="B119" s="98"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="90"/>
+      <c r="B120" s="98"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="90"/>
+      <c r="B121" s="98"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B122" s="90"/>
+      <c r="B122" s="98"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B123" s="90"/>
+      <c r="B123" s="98"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B124" s="90"/>
+      <c r="B124" s="98"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B125" s="90"/>
+      <c r="B125" s="98"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B126" s="90"/>
+      <c r="B126" s="98"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B127" s="90"/>
+      <c r="B127" s="98"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="90"/>
+      <c r="B128" s="98"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="90"/>
+      <c r="B129" s="98"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="90"/>
+      <c r="B130" s="98"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="90"/>
+      <c r="B131" s="98"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B132" s="90"/>
+      <c r="B132" s="98"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B133" s="90"/>
+      <c r="B133" s="98"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B134" s="90"/>
+      <c r="B134" s="98"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B135" s="90"/>
+      <c r="B135" s="98"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="90"/>
+      <c r="B136" s="98"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="90"/>
+      <c r="B137" s="98"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B138" s="90"/>
+      <c r="B138" s="98"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B139" s="90"/>
+      <c r="B139" s="98"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B140" s="90"/>
+      <c r="B140" s="98"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B141" s="90"/>
+      <c r="B141" s="98"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="90"/>
+      <c r="B142" s="98"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B143" s="90"/>
+      <c r="B143" s="98"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B144" s="90"/>
+      <c r="B144" s="98"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B145" s="90"/>
+      <c r="B145" s="98"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="90"/>
+      <c r="B146" s="98"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="90"/>
+      <c r="B147" s="98"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B148" s="90"/>
+      <c r="B148" s="98"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B149" s="90"/>
+      <c r="B149" s="98"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B150" s="90"/>
+      <c r="B150" s="98"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B151" s="90"/>
+      <c r="B151" s="98"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="90"/>
+      <c r="B152" s="98"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="90"/>
+      <c r="B153" s="98"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B154" s="90"/>
+      <c r="B154" s="98"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B155" s="90"/>
+      <c r="B155" s="98"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B156" s="90"/>
+      <c r="B156" s="98"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B157" s="90"/>
+      <c r="B157" s="98"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="90"/>
+      <c r="B158" s="98"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="90"/>
+      <c r="B159" s="98"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="90"/>
+      <c r="B160" s="98"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="90"/>
+      <c r="B161" s="98"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="90"/>
+      <c r="B162" s="98"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="90"/>
+      <c r="B163" s="98"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="90"/>
+      <c r="B164" s="98"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="90"/>
+      <c r="B165" s="98"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="90"/>
+      <c r="B166" s="98"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="90"/>
+      <c r="B167" s="98"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="90"/>
+      <c r="B168" s="98"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="90"/>
+      <c r="B169" s="98"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="90"/>
+      <c r="B170" s="98"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="90"/>
+      <c r="B171" s="98"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="90"/>
+      <c r="B172" s="98"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B173" s="90"/>
+      <c r="B173" s="98"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="90"/>
+      <c r="B174" s="98"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="90"/>
+      <c r="B175" s="98"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="90"/>
+      <c r="B176" s="98"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="90"/>
+      <c r="B177" s="98"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="90"/>
+      <c r="B178" s="98"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="90"/>
+      <c r="B179" s="98"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="90"/>
+      <c r="B180" s="98"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B181" s="90"/>
+      <c r="B181" s="98"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="90"/>
+      <c r="B182" s="98"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="90"/>
+      <c r="B183" s="98"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="90"/>
+      <c r="B184" s="98"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="90"/>
+      <c r="B185" s="98"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="90"/>
+      <c r="B186" s="98"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="90"/>
+      <c r="B187" s="98"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="90"/>
+      <c r="B188" s="98"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B189" s="90"/>
+      <c r="B189" s="98"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="90"/>
+      <c r="B190" s="98"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="90"/>
+      <c r="B191" s="98"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="90"/>
+      <c r="B192" s="98"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="90"/>
+      <c r="B193" s="98"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="90"/>
+      <c r="B194" s="98"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="90"/>
+      <c r="B195" s="98"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="90"/>
+      <c r="B196" s="98"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="90"/>
+      <c r="B197" s="98"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="90"/>
+      <c r="B198" s="98"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="90"/>
+      <c r="B199" s="98"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="90"/>
+      <c r="B200" s="98"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B201" s="90"/>
+      <c r="B201" s="98"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B202" s="90"/>
+      <c r="B202" s="98"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B203" s="90"/>
+      <c r="B203" s="98"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B204" s="90"/>
+      <c r="B204" s="98"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B205" s="90"/>
+      <c r="B205" s="98"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B206" s="90"/>
+      <c r="B206" s="98"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B207" s="90"/>
+      <c r="B207" s="98"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B208" s="90"/>
+      <c r="B208" s="98"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B209" s="90"/>
+      <c r="B209" s="98"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B210" s="90"/>
+      <c r="B210" s="98"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B211" s="90"/>
+      <c r="B211" s="98"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B212" s="90"/>
+      <c r="B212" s="98"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B213" s="90"/>
+      <c r="B213" s="98"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B214" s="90"/>
+      <c r="B214" s="98"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B215" s="90"/>
+      <c r="B215" s="98"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B216" s="90"/>
+      <c r="B216" s="98"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B217" s="90"/>
+      <c r="B217" s="98"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B218" s="90"/>
+      <c r="B218" s="98"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B219" s="90"/>
+      <c r="B219" s="98"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B220" s="90"/>
+      <c r="B220" s="98"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>